<commit_message>
Model3 has been added
</commit_message>
<xml_diff>
--- a/benchmarks/cscs2022/xlsx/Random/110.xlsx
+++ b/benchmarks/cscs2022/xlsx/Random/110.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnsai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PHD\P.h.D papers\Paper_Integer Programming Based Optimization of Power Consumption for DCNs\Solvers\New  benchmarks\New  benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB79137-B9E8-4F92-A564-122582C49B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F2224F-FDBA-4326-8317-7BF65B83412A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -680,7 +680,7 @@
   <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D109"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -696,7 +696,7 @@
         <v>16</v>
       </c>
       <c r="D1">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -738,7 +738,7 @@
         <v>16</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -752,7 +752,7 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -766,7 +766,7 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -780,7 +780,7 @@
         <v>15</v>
       </c>
       <c r="D7">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>16</v>
       </c>
       <c r="D8">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -808,7 +808,7 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -822,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -836,7 +836,7 @@
         <v>15</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -850,7 +850,7 @@
         <v>13</v>
       </c>
       <c r="D12">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,7 +864,7 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -878,7 +878,7 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -892,7 +892,7 @@
         <v>15</v>
       </c>
       <c r="D15">
-        <v>37</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -906,7 +906,7 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -934,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="D18">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -948,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -962,7 +962,7 @@
         <v>15</v>
       </c>
       <c r="D20">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -976,7 +976,7 @@
         <v>13</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
         <v>16</v>
       </c>
       <c r="D22">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1004,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="D23">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1018,7 +1018,7 @@
         <v>16</v>
       </c>
       <c r="D24">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1032,7 +1032,7 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1046,7 +1046,7 @@
         <v>16</v>
       </c>
       <c r="D26">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1060,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>16</v>
       </c>
       <c r="D28">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,7 +1088,7 @@
         <v>13</v>
       </c>
       <c r="D29">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1102,7 +1102,7 @@
         <v>15</v>
       </c>
       <c r="D30">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
         <v>14</v>
       </c>
       <c r="D31">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1130,7 +1130,7 @@
         <v>16</v>
       </c>
       <c r="D32">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1144,7 +1144,7 @@
         <v>16</v>
       </c>
       <c r="D33">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1158,7 +1158,7 @@
         <v>16</v>
       </c>
       <c r="D34">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
         <v>13</v>
       </c>
       <c r="D35">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1186,7 +1186,7 @@
         <v>13</v>
       </c>
       <c r="D36">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1200,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="D37">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1214,7 +1214,7 @@
         <v>14</v>
       </c>
       <c r="D38">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1228,7 +1228,7 @@
         <v>13</v>
       </c>
       <c r="D39">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,7 +1242,7 @@
         <v>14</v>
       </c>
       <c r="D40">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,7 +1256,7 @@
         <v>15</v>
       </c>
       <c r="D41">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1270,7 +1270,7 @@
         <v>15</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1284,7 +1284,7 @@
         <v>14</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,7 +1298,7 @@
         <v>13</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>16</v>
       </c>
       <c r="D45">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,7 +1326,7 @@
         <v>14</v>
       </c>
       <c r="D46">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1340,7 +1340,7 @@
         <v>16</v>
       </c>
       <c r="D47">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1354,7 +1354,7 @@
         <v>16</v>
       </c>
       <c r="D48">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1368,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="D49">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1382,7 +1382,7 @@
         <v>14</v>
       </c>
       <c r="D50">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1396,7 +1396,7 @@
         <v>14</v>
       </c>
       <c r="D51">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1410,7 +1410,7 @@
         <v>14</v>
       </c>
       <c r="D52">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1424,7 +1424,7 @@
         <v>16</v>
       </c>
       <c r="D53">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1438,7 +1438,7 @@
         <v>16</v>
       </c>
       <c r="D54">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1452,7 +1452,7 @@
         <v>13</v>
       </c>
       <c r="D55">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>16</v>
       </c>
       <c r="D56">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1480,7 +1480,7 @@
         <v>13</v>
       </c>
       <c r="D57">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="D58">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1508,7 +1508,7 @@
         <v>15</v>
       </c>
       <c r="D59">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
         <v>16</v>
       </c>
       <c r="D60">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,7 +1536,7 @@
         <v>14</v>
       </c>
       <c r="D61">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1550,7 +1550,7 @@
         <v>16</v>
       </c>
       <c r="D62">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,7 +1564,7 @@
         <v>13</v>
       </c>
       <c r="D63">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1578,7 +1578,7 @@
         <v>14</v>
       </c>
       <c r="D64">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,7 +1592,7 @@
         <v>16</v>
       </c>
       <c r="D65">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,7 +1606,7 @@
         <v>13</v>
       </c>
       <c r="D66">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1620,7 +1620,7 @@
         <v>13</v>
       </c>
       <c r="D67">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,7 +1634,7 @@
         <v>15</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1648,7 +1648,7 @@
         <v>14</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1662,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="D70">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1676,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="D71">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
         <v>14</v>
       </c>
       <c r="D72">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,7 +1704,7 @@
         <v>14</v>
       </c>
       <c r="D73">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1718,7 +1718,7 @@
         <v>16</v>
       </c>
       <c r="D74">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
         <v>16</v>
       </c>
       <c r="D75">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
         <v>14</v>
       </c>
       <c r="D76">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1760,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="D77">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1774,7 +1774,7 @@
         <v>14</v>
       </c>
       <c r="D78">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,7 +1788,7 @@
         <v>15</v>
       </c>
       <c r="D79">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,7 +1802,7 @@
         <v>13</v>
       </c>
       <c r="D80">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,7 +1816,7 @@
         <v>15</v>
       </c>
       <c r="D81">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
         <v>16</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,7 +1844,7 @@
         <v>15</v>
       </c>
       <c r="D83">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,7 +1858,7 @@
         <v>13</v>
       </c>
       <c r="D84">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,7 +1872,7 @@
         <v>15</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,7 +1886,7 @@
         <v>14</v>
       </c>
       <c r="D86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>15</v>
       </c>
       <c r="D87">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,7 +1914,7 @@
         <v>13</v>
       </c>
       <c r="D88">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,7 +1928,7 @@
         <v>13</v>
       </c>
       <c r="D89">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
         <v>14</v>
       </c>
       <c r="D90">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,7 +1956,7 @@
         <v>15</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -1970,7 +1970,7 @@
         <v>15</v>
       </c>
       <c r="D92">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -1984,7 +1984,7 @@
         <v>15</v>
       </c>
       <c r="D93">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1998,7 +1998,7 @@
         <v>16</v>
       </c>
       <c r="D94">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2012,7 +2012,7 @@
         <v>14</v>
       </c>
       <c r="D95">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2026,7 +2026,7 @@
         <v>16</v>
       </c>
       <c r="D96">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>15</v>
       </c>
       <c r="D97">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2054,7 +2054,7 @@
         <v>15</v>
       </c>
       <c r="D98">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2068,7 +2068,7 @@
         <v>14</v>
       </c>
       <c r="D99">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>16</v>
       </c>
       <c r="D100">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2096,7 +2096,7 @@
         <v>13</v>
       </c>
       <c r="D101">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,7 +2110,7 @@
         <v>16</v>
       </c>
       <c r="D102">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,7 +2124,7 @@
         <v>15</v>
       </c>
       <c r="D103">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2138,7 +2138,7 @@
         <v>16</v>
       </c>
       <c r="D104">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,7 +2152,7 @@
         <v>14</v>
       </c>
       <c r="D105">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2166,7 +2166,7 @@
         <v>13</v>
       </c>
       <c r="D106">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,7 +2180,7 @@
         <v>14</v>
       </c>
       <c r="D107">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
         <v>14</v>
       </c>
       <c r="D108">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2208,7 +2208,7 @@
         <v>15</v>
       </c>
       <c r="D109">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>